<commit_message>
fix: schedule alg fix, colors fix, groups fix, scroll fix
</commit_message>
<xml_diff>
--- a/python/table.xlsx
+++ b/python/table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -2265,22 +2265,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BD168"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AW1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AT119" activeCellId="0" sqref="AT119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="4" style="1" width="29.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="4" style="1" width="29.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>